<commit_message>
git update on 14th of April
</commit_message>
<xml_diff>
--- a/Data/Resultscomparison.xlsx
+++ b/Data/Resultscomparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UserA1\Documents\GitHub\Ordinal_Patterns_R\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809FEBB3-0534-4930-8634-34AF1A33A59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C0404D0-F546-4C53-B9B0-F467060C3D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8538A984-2847-4049-8566-959F13562AC3}"/>
+    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="12240" activeTab="2" xr2:uid="{8538A984-2847-4049-8566-959F13562AC3}"/>
   </bookViews>
   <sheets>
     <sheet name="48k&amp;NormalML0" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Batch Results_Normal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1321,17 +1322,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9A21F3-4C7F-4D48-80FB-D65B8EA40B4D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>284</v>
       </c>
@@ -1354,7 +1355,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>4.4147751508907801E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1419,16 +1420,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C130E44-524B-4210-95E8-A7532685F47D}">
   <dimension ref="A1:G255"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A238" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>284</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>6.0832207550848604E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>6.1463804047637597E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1520,7 +1521,7 @@
         <v>8.0374832473464903E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1543,7 +1544,7 @@
         <v>7.7782281278412297E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +1567,7 @@
         <v>7.2561498338054899E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>7.3844922638877999E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>7.4317303087956298E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>7.9924956605086396E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>7.9623509587034708E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1681,7 +1682,7 @@
         <v>8.0552114751419601E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1704,7 +1705,7 @@
         <v>7.8452623825216693E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>7.9201523535961001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1750,7 +1751,7 @@
         <v>5.8943385972235899E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>7.8910788298934501E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1796,7 +1797,7 @@
         <v>7.8227908187030893E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1819,7 +1820,7 @@
         <v>7.7736814936270101E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>7.5807719043690198E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1865,7 +1866,7 @@
         <v>7.4086409997629202E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>7.72584053873091E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>7.8775230752465997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1934,7 +1935,7 @@
         <v>7.3612394769598704E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>7.7601580821889098E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>7.9410734257016492E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>5.9354351035688299E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2026,7 +2027,7 @@
         <v>7.9671222313466399E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -2049,7 +2050,7 @@
         <v>7.4430437445181397E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -2072,7 +2073,7 @@
         <v>7.6271741961945402E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>7.2341568749963404E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>7.7295796921538701E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>7.5672948789261502E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -2164,7 +2165,7 @@
         <v>7.69904950417288E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>7.6097660951099603E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
@@ -2210,7 +2211,7 @@
         <v>7.3216974995368904E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
@@ -2233,7 +2234,7 @@
         <v>7.6163581294597304E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
@@ -2256,7 +2257,7 @@
         <v>6.1373352920981103E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -2279,7 +2280,7 @@
         <v>7.7142288346039901E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>7.4647006932460798E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>7.0823828326391398E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -2348,7 +2349,7 @@
         <v>7.2999075024016303E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>6.9426723171431802E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>45</v>
       </c>
@@ -2394,7 +2395,7 @@
         <v>7.2737848528122801E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>46</v>
       </c>
@@ -2417,7 +2418,7 @@
         <v>7.1137729211812103E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>47</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>7.3114675381861002E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>48</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>7.1444685053557999E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>49</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>7.1456212183259897E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>50</v>
       </c>
@@ -2509,7 +2510,7 @@
         <v>6.0544807707974104E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>6.89313838086251E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>7.1198568269963802E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
@@ -2578,7 +2579,7 @@
         <v>6.94749579363206E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>54</v>
       </c>
@@ -2601,7 +2602,7 @@
         <v>7.2448463436835201E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>55</v>
       </c>
@@ -2624,7 +2625,7 @@
         <v>7.3860535325893598E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>56</v>
       </c>
@@ -2647,7 +2648,7 @@
         <v>7.2251653447039004E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
@@ -2670,7 +2671,7 @@
         <v>7.2476703345531798E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>58</v>
       </c>
@@ -2693,7 +2694,7 @@
         <v>7.2927035208227896E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>59</v>
       </c>
@@ -2716,7 +2717,7 @@
         <v>7.4367718795230802E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>60</v>
       </c>
@@ -2739,7 +2740,7 @@
         <v>7.4366129058829403E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>61</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>6.2233840211687397E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>62</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>7.2785532885105602E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>63</v>
       </c>
@@ -2808,7 +2809,7 @@
         <v>7.1290857838881899E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>64</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>7.4423177101666897E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>65</v>
       </c>
@@ -2854,7 +2855,7 @@
         <v>6.9276012283469197E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>66</v>
       </c>
@@ -2877,7 +2878,7 @@
         <v>7.3542857267352799E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>67</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>7.0746234593567396E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>68</v>
       </c>
@@ -2923,7 +2924,7 @@
         <v>7.5169372115789501E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>69</v>
       </c>
@@ -2946,7 +2947,7 @@
         <v>6.86470651403922E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>70</v>
       </c>
@@ -2969,7 +2970,7 @@
         <v>7.1138164761674304E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>71</v>
       </c>
@@ -2992,7 +2993,7 @@
         <v>7.2359486693063003E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>72</v>
       </c>
@@ -3015,7 +3016,7 @@
         <v>5.6826814681503798E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>73</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>6.8847806399389699E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>74</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>7.0342060141793603E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>75</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>7.2208231009350298E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>76</v>
       </c>
@@ -3107,7 +3108,7 @@
         <v>7.0353078290027503E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>77</v>
       </c>
@@ -3130,7 +3131,7 @@
         <v>7.3154542623423196E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>78</v>
       </c>
@@ -3153,7 +3154,7 @@
         <v>7.3160495818939001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>79</v>
       </c>
@@ -3176,7 +3177,7 @@
         <v>7.0277849612368597E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>80</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>7.1841081635441902E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>7.0327363579115801E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>82</v>
       </c>
@@ -3245,7 +3246,7 @@
         <v>7.0508817412611403E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>83</v>
       </c>
@@ -3268,7 +3269,7 @@
         <v>6.0806385171972999E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>84</v>
       </c>
@@ -3291,7 +3292,7 @@
         <v>7.0917439702482604E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>85</v>
       </c>
@@ -3314,7 +3315,7 @@
         <v>7.2536192573236001E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -3337,7 +3338,7 @@
         <v>7.0325738072337003E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>87</v>
       </c>
@@ -3360,7 +3361,7 @@
         <v>7.2471760069547E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>88</v>
       </c>
@@ -3383,7 +3384,7 @@
         <v>7.1271765840796404E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>89</v>
       </c>
@@ -3406,7 +3407,7 @@
         <v>7.2403092285127403E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>90</v>
       </c>
@@ -3429,7 +3430,7 @@
         <v>6.9093403958220903E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>91</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>7.0267201754632101E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>92</v>
       </c>
@@ -3475,7 +3476,7 @@
         <v>7.0226542751105504E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>93</v>
       </c>
@@ -3498,7 +3499,7 @@
         <v>7.1388512294326004E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>94</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>6.0947300548790202E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>7.67775808162893E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
@@ -3567,7 +3568,7 @@
         <v>7.8344206228925604E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -3590,7 +3591,7 @@
         <v>7.3564865510436696E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>98</v>
       </c>
@@ -3613,7 +3614,7 @@
         <v>7.4717689885503901E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>99</v>
       </c>
@@ -3636,7 +3637,7 @@
         <v>7.2972657690665802E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
@@ -3659,7 +3660,7 @@
         <v>7.1669704816437101E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>101</v>
       </c>
@@ -3682,7 +3683,7 @@
         <v>7.62066884264293E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>102</v>
       </c>
@@ -3705,7 +3706,7 @@
         <v>7.6070110840204602E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>103</v>
       </c>
@@ -3728,7 +3729,7 @@
         <v>7.3159660044655704E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>104</v>
       </c>
@@ -3751,7 +3752,7 @@
         <v>7.4591706048301003E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>105</v>
       </c>
@@ -3774,7 +3775,7 @@
         <v>6.1373272566074503E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>106</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>7.2399272503386996E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>107</v>
       </c>
@@ -3820,7 +3821,7 @@
         <v>7.1484905676315897E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>108</v>
       </c>
@@ -3843,7 +3844,7 @@
         <v>7.8669251399308901E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>109</v>
       </c>
@@ -3866,7 +3867,7 @@
         <v>7.50556295635802E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>110</v>
       </c>
@@ -3889,7 +3890,7 @@
         <v>7.5207326123613904E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>111</v>
       </c>
@@ -3912,7 +3913,7 @@
         <v>7.6927058577701303E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>112</v>
       </c>
@@ -3935,7 +3936,7 @@
         <v>7.1129054438812704E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>113</v>
       </c>
@@ -3958,7 +3959,7 @@
         <v>7.6074638759033898E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>114</v>
       </c>
@@ -3981,7 +3982,7 @@
         <v>7.4985638853473499E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>115</v>
       </c>
@@ -4004,7 +4005,7 @@
         <v>7.3196719806574396E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>116</v>
       </c>
@@ -4027,7 +4028,7 @@
         <v>6.1430312849264602E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>117</v>
       </c>
@@ -4050,7 +4051,7 @@
         <v>6.0249891375718104E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>118</v>
       </c>
@@ -4073,7 +4074,7 @@
         <v>7.4854312113084203E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>119</v>
       </c>
@@ -4096,7 +4097,7 @@
         <v>7.5913798833053296E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>120</v>
       </c>
@@ -4119,7 +4120,7 @@
         <v>7.7212946342287599E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>121</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>7.6291216746209103E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>122</v>
       </c>
@@ -4165,7 +4166,7 @@
         <v>7.1851037398761898E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>123</v>
       </c>
@@ -4188,7 +4189,7 @@
         <v>7.3992318711088101E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>124</v>
       </c>
@@ -4211,7 +4212,7 @@
         <v>7.1062676592292496E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>125</v>
       </c>
@@ -4234,7 +4235,7 @@
         <v>7.4093300588798199E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>126</v>
       </c>
@@ -4257,7 +4258,7 @@
         <v>7.0749402863275399E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>127</v>
       </c>
@@ -4280,7 +4281,7 @@
         <v>7.3679199004654502E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>128</v>
       </c>
@@ -4303,7 +4304,7 @@
         <v>5.7601504269844802E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>129</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>7.2745784433624703E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>130</v>
       </c>
@@ -4349,7 +4350,7 @@
         <v>7.0729583909627204E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>131</v>
       </c>
@@ -4372,7 +4373,7 @@
         <v>7.3508558142011404E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>132</v>
       </c>
@@ -4395,7 +4396,7 @@
         <v>7.3707671632368297E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>133</v>
       </c>
@@ -4418,7 +4419,7 @@
         <v>7.3765956054543504E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>134</v>
       </c>
@@ -4441,7 +4442,7 @@
         <v>7.2182624771580297E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>135</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>7.4040044124735298E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>136</v>
       </c>
@@ -4487,7 +4488,7 @@
         <v>7.5789178650714903E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>137</v>
       </c>
@@ -4510,7 +4511,7 @@
         <v>6.9938381355605303E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>138</v>
       </c>
@@ -4533,7 +4534,7 @@
         <v>7.21476155418963E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>139</v>
       </c>
@@ -4556,7 +4557,7 @@
         <v>5.77214167566903E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>140</v>
       </c>
@@ -4579,7 +4580,7 @@
         <v>6.9687290919178803E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>141</v>
       </c>
@@ -4602,7 +4603,7 @@
         <v>6.9078385411449903E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>142</v>
       </c>
@@ -4625,7 +4626,7 @@
         <v>7.3253429429331902E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>143</v>
       </c>
@@ -4648,7 +4649,7 @@
         <v>7.0427799392010701E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>144</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>7.1589021308283204E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>145</v>
       </c>
@@ -4694,7 +4695,7 @@
         <v>7.3709280130520296E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>146</v>
       </c>
@@ -4717,7 +4718,7 @@
         <v>7.5257043273682196E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>147</v>
       </c>
@@ -4740,7 +4741,7 @@
         <v>7.1035206949184096E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>148</v>
       </c>
@@ -4763,7 +4764,7 @@
         <v>7.2034742817261698E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
@@ -4786,7 +4787,7 @@
         <v>7.0133921081712404E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -4809,7 +4810,7 @@
         <v>5.8733557161649097E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>151</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>7.2603060723721103E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>152</v>
       </c>
@@ -4855,7 +4856,7 @@
         <v>7.4249140537336403E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>153</v>
       </c>
@@ -4878,7 +4879,7 @@
         <v>6.9190415974137902E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>154</v>
       </c>
@@ -4901,7 +4902,7 @@
         <v>6.9936437834736999E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>155</v>
       </c>
@@ -4924,7 +4925,7 @@
         <v>6.9260427202644196E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>156</v>
       </c>
@@ -4947,7 +4948,7 @@
         <v>7.0660640234539501E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>157</v>
       </c>
@@ -4970,7 +4971,7 @@
         <v>7.13988772713241E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>158</v>
       </c>
@@ -4993,7 +4994,7 @@
         <v>7.17441808215566E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>159</v>
       </c>
@@ -5016,7 +5017,7 @@
         <v>6.8550304749838298E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>160</v>
       </c>
@@ -5039,7 +5040,7 @@
         <v>6.8446783041749802E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>161</v>
       </c>
@@ -5062,7 +5063,7 @@
         <v>6.1518426714103798E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>162</v>
       </c>
@@ -5085,7 +5086,7 @@
         <v>7.0817696077905999E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>163</v>
       </c>
@@ -5108,7 +5109,7 @@
         <v>7.2143574600390297E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>164</v>
       </c>
@@ -5131,7 +5132,7 @@
         <v>6.7562146170820304E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>165</v>
       </c>
@@ -5154,7 +5155,7 @@
         <v>6.9725054164760901E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>166</v>
       </c>
@@ -5177,7 +5178,7 @@
         <v>6.8873092683266997E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>167</v>
       </c>
@@ -5200,7 +5201,7 @@
         <v>6.81729357145479E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>168</v>
       </c>
@@ -5223,7 +5224,7 @@
         <v>6.7860221726715603E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>169</v>
       </c>
@@ -5246,7 +5247,7 @@
         <v>7.2517468504251304E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>170</v>
       </c>
@@ -5269,7 +5270,7 @@
         <v>6.9397613518872199E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>171</v>
       </c>
@@ -5292,7 +5293,7 @@
         <v>7.1757064838305499E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>172</v>
       </c>
@@ -5315,7 +5316,7 @@
         <v>6.5472119706478796E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>173</v>
       </c>
@@ -5338,7 +5339,7 @@
         <v>7.0021479318438202E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>174</v>
       </c>
@@ -5361,7 +5362,7 @@
         <v>7.37162779279848E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>175</v>
       </c>
@@ -5384,7 +5385,7 @@
         <v>6.6657280047240901E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>176</v>
       </c>
@@ -5407,7 +5408,7 @@
         <v>6.9013229130643096E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>177</v>
       </c>
@@ -5430,7 +5431,7 @@
         <v>7.3135183859677497E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>178</v>
       </c>
@@ -5453,7 +5454,7 @@
         <v>6.3547980070076202E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>179</v>
       </c>
@@ -5476,7 +5477,7 @@
         <v>6.6758804888696196E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>180</v>
       </c>
@@ -5499,7 +5500,7 @@
         <v>6.7467414106270702E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>181</v>
       </c>
@@ -5522,7 +5523,7 @@
         <v>6.4542357957717098E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>182</v>
       </c>
@@ -5545,7 +5546,7 @@
         <v>6.0175273248052503E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>183</v>
       </c>
@@ -5568,7 +5569,7 @@
         <v>6.5131367901065601E-3</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>184</v>
       </c>
@@ -5591,7 +5592,7 @@
         <v>6.3013690046184101E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>185</v>
       </c>
@@ -5614,7 +5615,7 @@
         <v>6.8806060929047499E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>186</v>
       </c>
@@ -5637,7 +5638,7 @@
         <v>6.6547611086589797E-3</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>187</v>
       </c>
@@ -5660,7 +5661,7 @@
         <v>6.5584028702410802E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>188</v>
       </c>
@@ -5683,7 +5684,7 @@
         <v>6.42896666455993E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>189</v>
       </c>
@@ -5706,7 +5707,7 @@
         <v>6.5802624104455004E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>190</v>
       </c>
@@ -5729,7 +5730,7 @@
         <v>6.6112946669361601E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>191</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>6.5657791767903999E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>192</v>
       </c>
@@ -5775,7 +5776,7 @@
         <v>6.5415923586681904E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>193</v>
       </c>
@@ -5798,7 +5799,7 @@
         <v>6.2526268206045E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>194</v>
       </c>
@@ -5821,7 +5822,7 @@
         <v>6.4528248757628401E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>195</v>
       </c>
@@ -5844,7 +5845,7 @@
         <v>6.47842171263854E-3</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>196</v>
       </c>
@@ -5867,7 +5868,7 @@
         <v>6.5794102237772796E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>197</v>
       </c>
@@ -5890,7 +5891,7 @@
         <v>6.5951330093151801E-3</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>198</v>
       </c>
@@ -5913,7 +5914,7 @@
         <v>6.5899851270367999E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>199</v>
       </c>
@@ -5936,7 +5937,7 @@
         <v>6.6601639931199996E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>200</v>
       </c>
@@ -5959,7 +5960,7 @@
         <v>6.6687117339217401E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>201</v>
       </c>
@@ -5982,7 +5983,7 @@
         <v>6.5590894083240904E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>202</v>
       </c>
@@ -6005,7 +6006,7 @@
         <v>6.7495539101180696E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>203</v>
       </c>
@@ -6028,7 +6029,7 @@
         <v>6.35583953933042E-3</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>204</v>
       </c>
@@ -6051,7 +6052,7 @@
         <v>6.2200358899771498E-3</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>205</v>
       </c>
@@ -6074,7 +6075,7 @@
         <v>5.8619854889646102E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>206</v>
       </c>
@@ -6097,7 +6098,7 @@
         <v>6.0494268279892398E-3</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>207</v>
       </c>
@@ -6120,7 +6121,7 @@
         <v>5.9486209864841504E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>208</v>
       </c>
@@ -6143,7 +6144,7 @@
         <v>5.8768960679949104E-3</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>209</v>
       </c>
@@ -6166,7 +6167,7 @@
         <v>5.8327399306238696E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>210</v>
       </c>
@@ -6189,7 +6190,7 @@
         <v>5.9042900714714498E-3</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>211</v>
       </c>
@@ -6212,7 +6213,7 @@
         <v>5.9276013399337897E-3</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>212</v>
       </c>
@@ -6235,7 +6236,7 @@
         <v>5.8052487211074401E-3</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>213</v>
       </c>
@@ -6258,7 +6259,7 @@
         <v>5.8734315607377498E-3</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>214</v>
       </c>
@@ -6281,7 +6282,7 @@
         <v>6.0203804398170401E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>215</v>
       </c>
@@ -6304,7 +6305,7 @@
         <v>5.8895123989792901E-3</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>216</v>
       </c>
@@ -6327,7 +6328,7 @@
         <v>6.1287074123477598E-3</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>217</v>
       </c>
@@ -6350,7 +6351,7 @@
         <v>6.1859641658629097E-3</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>218</v>
       </c>
@@ -6373,7 +6374,7 @@
         <v>6.1415614770267898E-3</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>219</v>
       </c>
@@ -6396,7 +6397,7 @@
         <v>5.9129180470796801E-3</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>220</v>
       </c>
@@ -6419,7 +6420,7 @@
         <v>5.9959935125196298E-3</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>221</v>
       </c>
@@ -6442,7 +6443,7 @@
         <v>5.88672973979203E-3</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>222</v>
       </c>
@@ -6465,7 +6466,7 @@
         <v>5.9518057546193003E-3</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>223</v>
       </c>
@@ -6488,7 +6489,7 @@
         <v>5.9634898077598197E-3</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>224</v>
       </c>
@@ -6511,7 +6512,7 @@
         <v>5.8744846582004899E-3</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>225</v>
       </c>
@@ -6534,7 +6535,7 @@
         <v>6.0026165290927901E-3</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>226</v>
       </c>
@@ -6557,7 +6558,7 @@
         <v>6.4620049360833397E-3</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>227</v>
       </c>
@@ -6580,7 +6581,7 @@
         <v>5.9064610735201899E-3</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>228</v>
       </c>
@@ -6603,7 +6604,7 @@
         <v>5.9832046453825597E-3</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>229</v>
       </c>
@@ -6626,7 +6627,7 @@
         <v>5.8524081419185602E-3</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>230</v>
       </c>
@@ -6649,7 +6650,7 @@
         <v>6.0523978550574504E-3</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>231</v>
       </c>
@@ -6672,7 +6673,7 @@
         <v>6.4053933687531397E-3</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>232</v>
       </c>
@@ -6695,7 +6696,7 @@
         <v>6.4579649980603298E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>233</v>
       </c>
@@ -6718,7 +6719,7 @@
         <v>6.4543359459558703E-3</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>234</v>
       </c>
@@ -6741,7 +6742,7 @@
         <v>6.6225677723177204E-3</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>235</v>
       </c>
@@ -6764,7 +6765,7 @@
         <v>6.5047765037400899E-3</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>236</v>
       </c>
@@ -6787,7 +6788,7 @@
         <v>6.4931065243026597E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>237</v>
       </c>
@@ -6810,7 +6811,7 @@
         <v>6.0036946925660197E-3</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>238</v>
       </c>
@@ -6833,7 +6834,7 @@
         <v>6.48730434534077E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>239</v>
       </c>
@@ -6856,7 +6857,7 @@
         <v>6.4243984972776101E-3</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>240</v>
       </c>
@@ -6879,7 +6880,7 @@
         <v>6.4364183992628903E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>241</v>
       </c>
@@ -6902,7 +6903,7 @@
         <v>6.8076701033832603E-3</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>242</v>
       </c>
@@ -6925,7 +6926,7 @@
         <v>6.6629756052914704E-3</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>243</v>
       </c>
@@ -6948,7 +6949,7 @@
         <v>6.4666296399902099E-3</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>244</v>
       </c>
@@ -6971,7 +6972,7 @@
         <v>6.9738278257510901E-3</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>245</v>
       </c>
@@ -6994,7 +6995,7 @@
         <v>7.8615460755010191E-3</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>246</v>
       </c>
@@ -7017,7 +7018,7 @@
         <v>7.7829034624459798E-3</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>247</v>
       </c>
@@ -7040,7 +7041,7 @@
         <v>7.93921786273241E-3</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>248</v>
       </c>
@@ -7063,7 +7064,7 @@
         <v>6.04940453710252E-3</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>249</v>
       </c>
@@ -7086,7 +7087,7 @@
         <v>7.8649886914270908E-3</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>250</v>
       </c>
@@ -7109,7 +7110,7 @@
         <v>7.8155782074502602E-3</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>251</v>
       </c>
@@ -7132,7 +7133,7 @@
         <v>7.7350308001008696E-3</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>252</v>
       </c>
@@ -7155,7 +7156,7 @@
         <v>7.64659860069636E-3</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>253</v>
       </c>
@@ -7178,7 +7179,7 @@
         <v>7.7153633242870003E-3</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>254</v>
       </c>
@@ -7201,7 +7202,7 @@
         <v>7.8925719437198394E-3</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>255</v>
       </c>
@@ -7224,7 +7225,7 @@
         <v>7.9072396002418804E-3</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>256</v>
       </c>
@@ -7247,7 +7248,7 @@
         <v>7.4356747933505898E-3</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>257</v>
       </c>
@@ -7270,7 +7271,7 @@
         <v>7.77816605521331E-3</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>258</v>
       </c>
@@ -7312,16 +7313,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5779615-B7BE-4E88-97D9-169F01151F72}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>284</v>
       </c>
@@ -7344,7 +7345,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>259</v>
       </c>
@@ -7367,7 +7368,7 @@
         <v>6.3660404139475497E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>260</v>
       </c>
@@ -7390,7 +7391,7 @@
         <v>6.4440479611416104E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>261</v>
       </c>
@@ -7413,7 +7414,7 @@
         <v>6.5921728072458703E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>262</v>
       </c>
@@ -7436,7 +7437,7 @@
         <v>6.7102769858262403E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>263</v>
       </c>
@@ -7459,7 +7460,7 @@
         <v>6.7544323410474198E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>264</v>
       </c>
@@ -7482,7 +7483,7 @@
         <v>6.3751139412684997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>265</v>
       </c>
@@ -7505,7 +7506,7 @@
         <v>6.3513545465490899E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>266</v>
       </c>
@@ -7528,7 +7529,7 @@
         <v>6.6857202261397198E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>267</v>
       </c>
@@ -7551,7 +7552,7 @@
         <v>6.3308269012929304E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>268</v>
       </c>
@@ -7574,7 +7575,7 @@
         <v>6.2480958411164104E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>269</v>
       </c>
@@ -7597,7 +7598,7 @@
         <v>6.5062840661751498E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>270</v>
       </c>
@@ -7620,7 +7621,7 @@
         <v>6.2966603750363101E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>271</v>
       </c>
@@ -7643,7 +7644,7 @@
         <v>6.27721709284647E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>272</v>
       </c>
@@ -7666,7 +7667,7 @@
         <v>6.20522220358064E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>273</v>
       </c>
@@ -7689,7 +7690,7 @@
         <v>6.1268842512358602E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>274</v>
       </c>
@@ -7712,7 +7713,7 @@
         <v>6.1685262647511096E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>275</v>
       </c>
@@ -7735,7 +7736,7 @@
         <v>6.5250244171240496E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>276</v>
       </c>
@@ -7758,7 +7759,7 @@
         <v>9.8398585539981494E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>277</v>
       </c>
@@ -7781,7 +7782,7 @@
         <v>6.2895864512038102E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>278</v>
       </c>
@@ -7804,7 +7805,7 @@
         <v>6.1704604459220901E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>279</v>
       </c>
@@ -7827,7 +7828,7 @@
         <v>6.2234451825460002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>280</v>
       </c>
@@ -7850,7 +7851,7 @@
         <v>6.5501762368052304E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>281</v>
       </c>
@@ -7873,7 +7874,7 @@
         <v>6.17370847707574E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>282</v>
       </c>
@@ -7896,7 +7897,7 @@
         <v>6.0872491251544297E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>283</v>
       </c>
@@ -7920,8 +7921,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:G26">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="A1:G1">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -7930,8 +7931,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:G1">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="A2:G26">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>